<commit_message>
docs(Ver. 0.6.0.0 - beta): 📚Stocket - Docs
DOCS: Se ha añadido bitácora 9 y sus evidencias
</commit_message>
<xml_diff>
--- a/docs/manuales/Matriz de Trazabilidad.xlsx
+++ b/docs/manuales/Matriz de Trazabilidad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\PycharmProjects\Stocket\docs\manuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEDEA80-DF14-4B8C-8CF3-EE9C057B7F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73452739-3460-4AA7-9F72-274FB08FAA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,13 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
-    <t>UNIDAD MEDICA RADIOLOGICA DEL CARMEN</t>
-  </si>
-  <si>
     <t>Nombre del Proyecto:</t>
-  </si>
-  <si>
-    <t>Analisis y desarrollo de un sistema de asignación e inventario para la oficina de sistemas de la Unidad Médica Radiológica del Carmen – Sede Principal (Riohacha)</t>
   </si>
   <si>
     <t>Descripción:</t>
@@ -250,6 +244,12 @@
   </si>
   <si>
     <t>Archivos en extencion .html, .vue, .ts y .py</t>
+  </si>
+  <si>
+    <t>Stocket</t>
+  </si>
+  <si>
+    <t>Sistema de Gestion y Asignacion de elementos TI empresarial.</t>
   </si>
 </sst>
 </file>
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -802,7 +802,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -831,10 +831,10 @@
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -862,10 +862,10 @@
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -893,37 +893,37 @@
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -942,37 +942,37 @@
     </row>
     <row r="5" spans="1:26" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="F5" s="7">
         <v>44732</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="10"/>
@@ -992,37 +992,37 @@
     </row>
     <row r="6" spans="1:26" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="7">
         <v>44732</v>
       </c>
       <c r="G6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="K6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="10"/>
@@ -1042,37 +1042,37 @@
     </row>
     <row r="7" spans="1:26" s="11" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7">
         <v>44732</v>
       </c>
       <c r="G7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="K7" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="10"/>
@@ -1092,37 +1092,37 @@
     </row>
     <row r="8" spans="1:26" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" s="7">
         <v>44732</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="K8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="10"/>
@@ -1142,37 +1142,37 @@
     </row>
     <row r="9" spans="1:26" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F9" s="7">
         <v>44732</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="10"/>
@@ -1192,37 +1192,37 @@
     </row>
     <row r="10" spans="1:26" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10" s="7">
         <v>44732</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="10"/>
@@ -1242,37 +1242,37 @@
     </row>
     <row r="11" spans="1:26" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F11" s="7">
         <v>44732</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="K11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="10"/>
@@ -1292,37 +1292,37 @@
     </row>
     <row r="12" spans="1:26" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F12" s="7">
         <v>44732</v>
       </c>
       <c r="G12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="K12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="10"/>
@@ -1342,37 +1342,37 @@
     </row>
     <row r="13" spans="1:26" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="E13" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" s="7">
         <v>44732</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="K13" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="10"/>
@@ -1392,37 +1392,37 @@
     </row>
     <row r="14" spans="1:26" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" s="7">
         <v>44732</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="10"/>

</xml_diff>